<commit_message>
adding more data sources
</commit_message>
<xml_diff>
--- a/source/GP-figures.xlsx
+++ b/source/GP-figures.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="17820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32580" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General Program - Figures" sheetId="1" r:id="rId1"/>
@@ -21,49 +21,49 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Year</t>
+    <t>applications</t>
   </si>
   <si>
-    <t># of Grant applications</t>
+    <t>approved</t>
   </si>
   <si>
-    <t># of Grants approved</t>
+    <t>dollars mn</t>
   </si>
   <si>
-    <t>$ amount Grants MN</t>
+    <t>dollars nyc</t>
   </si>
   <si>
-    <t>$ amount Grants NYC</t>
+    <t>dollars other</t>
   </si>
   <si>
-    <t>$ amount Grants other</t>
+    <t>genre-Visual Arts</t>
   </si>
   <si>
-    <t># Visual Arts</t>
+    <t>genre-Theater</t>
   </si>
   <si>
-    <t># Theater</t>
+    <t>genre-Dance</t>
   </si>
   <si>
-    <t># Dance</t>
+    <t>genre-Media Arts/Film and Video</t>
   </si>
   <si>
-    <t># Media Arts/Film and Video</t>
+    <t>genre-Multidisciplinary</t>
   </si>
   <si>
-    <t># Multidisciplinary</t>
+    <t>genre-Literature</t>
   </si>
   <si>
-    <t># Literature</t>
+    <t>genre-Music</t>
   </si>
   <si>
-    <t># Music</t>
+    <t>genre-Arts Criticism</t>
   </si>
   <si>
-    <t># Arts Criticism</t>
+    <t>genre-Other Disciplines</t>
   </si>
   <si>
-    <t># Other Disciplines</t>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -79,7 +79,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -118,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -135,6 +134,7 @@
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +470,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -490,51 +490,51 @@
     <col min="15" max="15" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="60">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="80">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -547,13 +547,13 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <v>32684.84</v>
       </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
         <v>6822</v>
       </c>
       <c r="G2">
@@ -594,13 +594,13 @@
       <c r="C3">
         <v>6</v>
       </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
         <v>54000</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>10654.41</v>
       </c>
       <c r="G3">
@@ -641,13 +641,13 @@
       <c r="C4">
         <v>12</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <v>14000</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="8">
         <v>24000</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>33750</v>
       </c>
       <c r="G4">
@@ -688,13 +688,13 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>18610</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="8">
         <v>33500</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>115405</v>
       </c>
       <c r="G5">
@@ -735,13 +735,13 @@
       <c r="C6">
         <v>20</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>6380</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="8">
         <v>95000</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>60000</v>
       </c>
       <c r="G6">
@@ -782,13 +782,13 @@
       <c r="C7">
         <v>18</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>3650</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>543000</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>13250</v>
       </c>
       <c r="G7">
@@ -829,13 +829,13 @@
       <c r="C8">
         <v>19</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>33898</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="8">
         <v>452500</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
         <v>46000</v>
       </c>
       <c r="G8">
@@ -876,13 +876,13 @@
       <c r="C9">
         <v>13</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <v>54940</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="8">
         <v>120000</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="8">
         <v>50332</v>
       </c>
       <c r="G9">
@@ -923,13 +923,13 @@
       <c r="C10">
         <v>11</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="8">
         <v>16400</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="8">
         <v>132000</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="8">
         <v>86000</v>
       </c>
       <c r="G10">
@@ -970,13 +970,13 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="8">
         <v>109100</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="8">
         <v>170900</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="8">
         <v>14875</v>
       </c>
       <c r="G11">
@@ -1017,13 +1017,13 @@
       <c r="C12">
         <v>48</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="8">
         <v>352809</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="8">
         <v>524144</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="8">
         <v>56975</v>
       </c>
       <c r="G12">
@@ -1064,13 +1064,13 @@
       <c r="C13">
         <v>37</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="8">
         <v>346610</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <v>188245</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="8">
         <v>31292</v>
       </c>
       <c r="G13">
@@ -1111,13 +1111,13 @@
       <c r="C14">
         <v>63</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="8">
         <v>541875</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="8">
         <v>294950</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="8">
         <v>65554</v>
       </c>
       <c r="G14">
@@ -1158,13 +1158,13 @@
       <c r="C15">
         <v>70</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="8">
         <v>452824</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="8">
         <v>325325</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="8">
         <v>71863</v>
       </c>
       <c r="G15">
@@ -1205,13 +1205,13 @@
       <c r="C16">
         <v>53</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="8">
         <v>275465</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="8">
         <v>220298</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="8">
         <v>75200</v>
       </c>
       <c r="G16">
@@ -1252,13 +1252,13 @@
       <c r="C17">
         <v>63</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="8">
         <v>349318</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="8">
         <v>234572.13</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="8">
         <v>93300</v>
       </c>
       <c r="G17">
@@ -1299,13 +1299,13 @@
       <c r="C18">
         <v>64</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <v>470521.27</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <v>191597.87</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="8">
         <v>41628</v>
       </c>
       <c r="G18">
@@ -1346,13 +1346,13 @@
       <c r="C19">
         <v>70</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="8">
         <v>423673.41</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="8">
         <v>386484.33</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="8">
         <v>72604</v>
       </c>
       <c r="G19">
@@ -1393,13 +1393,13 @@
       <c r="C20">
         <v>70</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="8">
         <v>641557.49</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="8">
         <v>360030</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="8">
         <v>79926.009999999995</v>
       </c>
       <c r="G20">
@@ -1440,13 +1440,13 @@
       <c r="C21">
         <v>75</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="8">
         <v>640579.97</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="8">
         <v>411100</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="8">
         <v>19447</v>
       </c>
       <c r="G21">
@@ -1487,13 +1487,13 @@
       <c r="C22">
         <v>81</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="8">
         <v>1054592</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="8">
         <v>520650</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="8">
         <v>19826</v>
       </c>
       <c r="G22">
@@ -1534,13 +1534,13 @@
       <c r="C23">
         <v>75</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>720848</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="8">
         <v>406700</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="8">
         <v>36810</v>
       </c>
       <c r="G23">
@@ -1581,13 +1581,13 @@
       <c r="C24">
         <v>91</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="8">
         <v>790420</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="8">
         <v>402150</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="8">
         <v>46333</v>
       </c>
       <c r="G24">
@@ -1628,13 +1628,13 @@
       <c r="C25">
         <v>93</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="8">
         <v>925930.11</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="8">
         <v>540105</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="8">
         <v>46070</v>
       </c>
       <c r="G25">
@@ -1675,13 +1675,13 @@
       <c r="C26">
         <v>85</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="8">
         <v>987922.21</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="8">
         <v>519330</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="8">
         <v>25203</v>
       </c>
       <c r="G26">
@@ -1722,13 +1722,13 @@
       <c r="C27">
         <v>87</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="8">
         <v>1015105</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="8">
         <v>576200</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="8">
         <v>27182</v>
       </c>
       <c r="G27">
@@ -1769,13 +1769,13 @@
       <c r="C28">
         <v>89</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="8">
         <v>710453</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="8">
         <v>698200</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="8">
         <v>15502</v>
       </c>
       <c r="G28">
@@ -1816,13 +1816,13 @@
       <c r="C29">
         <v>86</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="8">
         <v>979755</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="8">
         <v>525700</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="8">
         <v>37899</v>
       </c>
       <c r="G29">
@@ -1863,13 +1863,13 @@
       <c r="C30">
         <v>96</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="8">
         <v>699191</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="8">
         <v>536200</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="8">
         <v>28188</v>
       </c>
       <c r="G30">
@@ -1910,13 +1910,13 @@
       <c r="C31">
         <v>93</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="8">
         <v>1170700</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="8">
         <v>702550</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="8">
         <v>23886</v>
       </c>
       <c r="G31">
@@ -1957,13 +1957,13 @@
       <c r="C32">
         <v>87</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="8">
         <v>854886</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="8">
         <v>537700</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="8">
         <v>7930</v>
       </c>
       <c r="G32">
@@ -2004,13 +2004,13 @@
       <c r="C33">
         <v>111</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="8">
         <v>1409650</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="8">
         <v>771000</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="8">
         <v>9831</v>
       </c>
       <c r="G33">
@@ -2051,13 +2051,13 @@
       <c r="C34">
         <v>97</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="8">
         <v>1088515</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="8">
         <v>564460</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="8">
         <v>9512</v>
       </c>
       <c r="G34">
@@ -2098,13 +2098,13 @@
       <c r="C35">
         <v>120</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="8">
         <v>1839140</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="8">
         <v>916100</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="8">
         <v>14870</v>
       </c>
       <c r="G35">
@@ -2145,13 +2145,13 @@
       <c r="C36">
         <v>136</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="8">
         <v>1614430</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="8">
         <v>1354650</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="8">
         <v>43856</v>
       </c>
       <c r="G36">
@@ -2192,13 +2192,13 @@
       <c r="C37">
         <v>120</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="8">
         <v>1953397</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="8">
         <v>1210000</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="8">
         <v>22291</v>
       </c>
       <c r="G37">
@@ -2239,13 +2239,13 @@
       <c r="C38">
         <v>145</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="8">
         <v>2356046</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="8">
         <v>1753150</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="8">
         <v>37020</v>
       </c>
       <c r="G38">
@@ -2286,13 +2286,13 @@
       <c r="C39">
         <v>127</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="8">
         <v>1858200</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="8">
         <v>1396650</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="8">
         <v>22120</v>
       </c>
       <c r="G39">
@@ -2333,13 +2333,13 @@
       <c r="C40">
         <v>117</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="8">
         <v>1634550</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="8">
         <v>1467250</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="8">
         <v>21036</v>
       </c>
       <c r="G40">
@@ -2380,13 +2380,13 @@
       <c r="C41">
         <v>99</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="8">
         <v>1637440</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="8">
         <v>1308000</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="8">
         <v>19440</v>
       </c>
       <c r="G41">
@@ -2427,13 +2427,13 @@
       <c r="C42">
         <v>97</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="8">
         <v>1249674</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="8">
         <v>1176986</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="8">
         <v>17746</v>
       </c>
       <c r="G42">
@@ -2474,13 +2474,13 @@
       <c r="C43">
         <v>92</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="8">
         <v>1390250</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="8">
         <v>1063750</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F43" s="8">
         <v>27740</v>
       </c>
       <c r="G43">
@@ -2521,13 +2521,13 @@
       <c r="C44">
         <v>105</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="8">
         <v>1545025.48</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="8">
         <v>1456750</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F44" s="8">
         <v>37740</v>
       </c>
       <c r="G44">
@@ -2568,13 +2568,13 @@
       <c r="C45">
         <v>85</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="8">
         <v>1529900</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="8">
         <v>897250</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F45" s="8">
         <v>32170</v>
       </c>
       <c r="G45">
@@ -2615,13 +2615,13 @@
       <c r="C46">
         <v>89</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="8">
         <v>1019887</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="8">
         <v>1100035</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="8">
         <v>9830</v>
       </c>
       <c r="G46">
@@ -2662,13 +2662,13 @@
       <c r="C47">
         <v>81</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="8">
         <v>1062742</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="8">
         <v>701200</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="8">
         <v>23327</v>
       </c>
       <c r="G47">
@@ -2709,13 +2709,13 @@
       <c r="C48">
         <v>97</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="8">
         <v>1613065</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="8">
         <v>1139250</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="8">
         <v>32050</v>
       </c>
       <c r="G48">
@@ -2756,13 +2756,13 @@
       <c r="C49">
         <v>83</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="8">
         <v>1094005</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="8">
         <v>865650</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="8">
         <v>71280</v>
       </c>
       <c r="G49">
@@ -2803,13 +2803,13 @@
       <c r="C50">
         <v>82</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="8">
         <v>1425339</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="8">
         <v>1465570</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="8">
         <v>32000</v>
       </c>
       <c r="G50">
@@ -2850,13 +2850,13 @@
       <c r="C51">
         <v>78</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="8">
         <v>1135655</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="8">
         <v>840900</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="8">
         <v>25000</v>
       </c>
       <c r="G51">

</xml_diff>